<commit_message>
Add BLEU correct calculation scripts
</commit_message>
<xml_diff>
--- a/BLEU/azure_output_sheet/azure_output_2.xlsx
+++ b/BLEU/azure_output_sheet/azure_output_2.xlsx
@@ -1,46 +1,87 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\extract_raw-data\BLEU\azure_output_sheet\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94805A17-3798-4F02-AA7A-48A042479A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="2030" yWindow="3590" windowWidth="23570" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="工作表1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>致謝</t>
+  </si>
+  <si>
+    <t>Acknowledgments</t>
+  </si>
+  <si>
+    <t>Thanks</t>
+  </si>
+  <si>
+    <t>本譯者群首先要感謝未具名的文稿抄寫者，以及敦珠仁波切法教的錄音發行者。此外，我們特別欠楚璽仁波切一個人情，他仁慈地為本書作序並為這整個翻譯計畫給予加持。同時非常感謝我們的老師貝瑪旺嘉仁波切、吉美欽哲仁波切，尤其是禳卓仁波切，他於很多場合在文字上給予我們很大的幫助，讓這個翻譯得以完成。更要感謝我們的讀者珍妮．肯恩、史提夫．蓋辛及薇薇安．庫爾滋的慷慨協助和寶貴建議。此書譯者為蓮師翻譯小組的海蓮娜．布雷克雷德與伍斯坦．福萊徹。</t>
+  </si>
+  <si>
+    <t>The translators would like to thank, first of all, the anonymous transcriber and the publisher of the recordings of Dudjom Rinpoche’s teachings. In addition, we owe a special debt of gratitude to Trulshik Rinpoche, who graciously composed the preface to the book and gave his blessing to the entire project. We are also very grateful to our teachers Pema Wangyal Rinpoche, Jigme Khyentse Rinpoche, and especially Rangdrol Rinpoche, who on numerous occasions gave us much help with the text and generally made the translation possible. Last but not least, we would like to thank our readers, Jenny Kane, Steve Gethin, and Vivian Kurz, for their generous help and valuable suggestions. The translation was made by Helena Blankleder and Wulstan Fletcher of the Padmakara Translation Group.</t>
+  </si>
+  <si>
+    <t>The translators would like to thank the unnamed copyists of the manuscript and the publishers of the recordings of Dundrup Rinpoche. In addition, we owe a special favor to Chuxi Rinpoche, who graciously wrote the foreword to the book and blessed the entire translation project. We would also like to thank our teachers Pema Wanggyal Rinpoche, Jigme Khyentse Rinpoche and especially Rinpoche Chucho, who helped us a lot on many occasions in writing to make this translation possible. Thanks even more to our reader, Jenny. Ken, Steve. Gaisin and Vivian. Kulc's generous assistance and valuable advice. The translator of this book is Helena of the Lotus Translation Team. Blake Cred and Wustein. Fletccher.</t>
+  </si>
+  <si>
+    <t>蓮師翻譯小組同時要向參札基金會（Tsadra Foundation）的慷慨協助，以及對翻譯本書的贊助，表達深切感激。</t>
+  </si>
+  <si>
+    <t>The Padmakara Translation Group gratefully acknowledges the generous support of the Tsadra Foundation in sponsoring the translation of this book.</t>
+  </si>
+  <si>
+    <t>The Lotus Translation Team would also like to express its deep gratitude to the Tsadra Foundation for its generous assistance and sponsorship in translating this book.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="新細明體"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF839496"/>
       <name val="Courier New"/>
       <family val="3"/>
-      <color rgb="FF839496"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="9"/>
       <name val="新細明體"/>
+      <family val="3"/>
       <charset val="136"/>
-      <family val="3"/>
-      <sz val="9"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -59,83 +100,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -401,72 +383,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>致謝</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Acknowledgments</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Thanks</t>
-        </is>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>本譯者群首先要感謝未具名的文稿抄寫者，以及敦珠仁波切法教的錄音發行者。此外，我們特別欠楚璽仁波切一個人情，他仁慈地為本書作序並為這整個翻譯計畫給予加持。同時非常感謝我們的老師貝瑪旺嘉仁波切、吉美欽哲仁波切，尤其是禳卓仁波切，他於很多場合在文字上給予我們很大的幫助，讓這個翻譯得以完成。更要感謝我們的讀者珍妮．肯恩、史提夫．蓋辛及薇薇安．庫爾滋的慷慨協助和寶貴建議。此書譯者為蓮師翻譯小組的海蓮娜．布雷克雷德與伍斯坦．福萊徹。</t>
-        </is>
-      </c>
-      <c r="B2" s="1" t="inlineStr">
-        <is>
-          <t>The translators would like to thank, first of all, the anonymous transcriber and the publisher of the recordings of Dudjom Rinpoche’s teachings. In addition, we owe a special debt of gratitude to Trulshik Rinpoche, who graciously composed the preface to the book and gave his blessing to the entire project. We are also very grateful to our teachers Pema Wangyal Rinpoche, Jigme Khyentse Rinpoche, and especially Rangdrol Rinpoche, who on numerous occasions gave us much help with the text and generally made the translation possible. Last but not least, we would like to thank our readers, Jenny Kane, Steve Gethin, and Vivian Kurz, for their generous help and valuable suggestions. The translation was made by Helena Blankleder and Wulstan Fletcher of the Padmakara Translation Group.</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>The translators would like to thank the unnamed copyists of the manuscript and the publishers of the recordings of Dundrup Rinpoche. In addition, we owe a special favor to Chuxi Rinpoche, who graciously wrote the foreword to the book and blessed the entire translation project. We would also like to thank our teachers Pema Wanggyal Rinpoche, Jigme Khyentse Rinpoche and especially Rinpoche Chucho, who helped us a lot on many occasions in writing to make this translation possible. Thanks even more to our reader, Jenny. Ken, Steve. Gaisin and Vivian. Kulc's generous assistance and valuable advice. The translator of this book is Helena of the Lotus Translation Team. Blake Cred and Wustein. Fletccher.</t>
-        </is>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>蓮師翻譯小組同時要向參札基金會（Tsadra Foundation）的慷慨協助，以及對翻譯本書的贊助，表達深切感激。</t>
-        </is>
-      </c>
-      <c r="B3" s="1" t="inlineStr">
-        <is>
-          <t>The Padmakara Translation Group gratefully acknowledges the generous support of the Tsadra Foundation in sponsoring the translation of this book.</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>The Lotus Translation Team would also like to express its deep gratitude to the Tsadra Foundation for its generous assistance and sponsorship in translating this book.</t>
-        </is>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>